<commit_message>
Updating the slope and constant for RVR based on the assumption that MCFP is accurate.
</commit_message>
<xml_diff>
--- a/notes/baseline.xlsx
+++ b/notes/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27900" yWindow="320" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -577,7 +577,6 @@
         <v>75</v>
       </c>
       <c r="H3">
-        <f>G13</f>
         <v>0</v>
       </c>
       <c r="I3">
@@ -620,12 +619,11 @@
         <v>75</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H8" si="6">G14</f>
-        <v>-6.6487404887373014</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="3"/>
-        <v>6.1441047235638369E-2</v>
+        <v>5.6437839886930283E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="4"/>
@@ -663,12 +661,11 @@
         <v>75</v>
       </c>
       <c r="H5">
-        <f t="shared" si="6"/>
-        <v>-3.0730320599423888</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>5.2351974981580417E-2</v>
+        <v>5.0291349266465626E-2</v>
       </c>
       <c r="K5">
         <f t="shared" si="4"/>
@@ -706,12 +703,11 @@
         <v>75</v>
       </c>
       <c r="H6">
-        <f t="shared" si="6"/>
-        <v>-2.9741989205143051</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>4.7905755606526226E-2</v>
+        <v>4.6078468522030548E-2</v>
       </c>
       <c r="K6">
         <f t="shared" si="4"/>
@@ -749,12 +745,11 @@
         <v>75</v>
       </c>
       <c r="H7">
-        <f t="shared" si="6"/>
-        <v>-2.9928327755528366</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>4.469090430318437E-2</v>
+        <v>4.2975972322798719E-2</v>
       </c>
       <c r="K7">
         <f t="shared" si="4"/>
@@ -792,12 +787,11 @@
         <v>75</v>
       </c>
       <c r="H8">
-        <f t="shared" si="6"/>
-        <v>-3.0125244217001379</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>4.220540322658025E-2</v>
+        <v>4.0575603282400931E-2</v>
       </c>
       <c r="K8">
         <f t="shared" si="4"/>
@@ -833,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <f>80*B2</f>
+        <f t="shared" ref="B13:B19" si="6">80*B2</f>
         <v>293.11635775695675</v>
       </c>
       <c r="C13">
@@ -841,19 +835,20 @@
         <v>205.1814504298697</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <f t="shared" ref="D13:D19" si="7">(B13-C13)*0.0047</f>
+        <v>0.41329406443730915</v>
       </c>
       <c r="E13">
         <f>(D13-H2)/D2</f>
-        <v>8.0953563086360574E-3</v>
+        <v>4.7796610169491543E-4</v>
       </c>
       <c r="G13">
-        <f>D13-(D2*E13)</f>
+        <f t="shared" ref="G13:G19" si="8">D13-(D2*E13)</f>
         <v>0</v>
       </c>
       <c r="K13">
         <f>E13*0.5/I2</f>
-        <v>4.6666666666666662E-2</v>
+        <v>2.7552937629153943E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -861,15 +856,15 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <f>80*B3</f>
+        <f t="shared" si="6"/>
         <v>382.3848793079091</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C19" si="7">B14*0.7</f>
+        <f t="shared" ref="C14:C19" si="9">B14*0.7</f>
         <v>267.66941551553634</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D19" si="8">(B14-C14)*0.0047</f>
+        <f t="shared" si="7"/>
         <v>0.539162679824152</v>
       </c>
       <c r="E14">
@@ -877,12 +872,12 @@
         <v>6.372054642132057E-3</v>
       </c>
       <c r="G14">
-        <f>D14-(D3*E14)</f>
+        <f t="shared" si="8"/>
         <v>-6.6487404887373014</v>
       </c>
       <c r="K14">
         <f>E13/2</f>
-        <v>4.0476781543180287E-3</v>
+        <v>2.3898305084745771E-4</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -890,24 +885,24 @@
         <v>2</v>
       </c>
       <c r="B15">
-        <f>80*B4</f>
+        <f t="shared" si="6"/>
         <v>450.47310216858386</v>
       </c>
       <c r="C15">
+        <f t="shared" si="9"/>
+        <v>315.33117151800866</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="7"/>
-        <v>315.33117151800866</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="8"/>
         <v>0.63516707405770345</v>
       </c>
       <c r="E15">
         <f>0.035*I4+0.00064</f>
-        <v>2.7904366532473432E-3</v>
+        <v>2.6153243960425599E-3</v>
       </c>
       <c r="G15">
-        <f>D15-(D4*E15)</f>
-        <v>-3.0730320599423888</v>
+        <f t="shared" si="8"/>
+        <v>-2.8403261428365827</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -915,24 +910,24 @@
         <v>3</v>
       </c>
       <c r="B16">
-        <f>80*B5</f>
+        <f t="shared" si="6"/>
         <v>505.5288669797514</v>
       </c>
       <c r="C16">
+        <f t="shared" si="9"/>
+        <v>353.87020688582595</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="7"/>
-        <v>353.87020688582595</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="8"/>
         <v>0.71279570244144963</v>
       </c>
       <c r="E16">
         <f>0.035*I5+0.00064</f>
-        <v>2.4723191243553148E-3</v>
+        <v>2.4001972243262973E-3</v>
       </c>
       <c r="G16">
-        <f>D16-(D5*E16)</f>
-        <v>-2.9741989205143051</v>
+        <f t="shared" si="8"/>
+        <v>-2.8666427984163216</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -940,24 +935,24 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <f>80*B6</f>
+        <f t="shared" si="6"/>
         <v>551.74856346199954</v>
       </c>
       <c r="C17">
+        <f t="shared" si="9"/>
+        <v>386.22399442339963</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="7"/>
-        <v>386.22399442339963</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="8"/>
         <v>0.77796547448141962</v>
       </c>
       <c r="E17">
         <f>0.035*I6+0.00064</f>
-        <v>2.3167014462284179E-3</v>
+        <v>2.2527463982710693E-3</v>
       </c>
       <c r="G17">
-        <f>D17-(D6*E17)</f>
-        <v>-2.9928327755528366</v>
+        <f t="shared" si="8"/>
+        <v>-2.888735813334836</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -965,24 +960,24 @@
         <v>5</v>
       </c>
       <c r="B18">
-        <f>80*B7</f>
+        <f t="shared" si="6"/>
         <v>591.58007229244367</v>
       </c>
       <c r="C18">
+        <f t="shared" si="9"/>
+        <v>414.10605060471056</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="7"/>
-        <v>414.10605060471056</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="8"/>
         <v>0.83412790193234565</v>
       </c>
       <c r="E18">
         <f>0.035*I7+0.00064</f>
-        <v>2.2041816506114531E-3</v>
+        <v>2.1441590312979552E-3</v>
       </c>
       <c r="G18">
-        <f>D18-(D7*E18)</f>
-        <v>-3.0125244217001379</v>
+        <f t="shared" si="8"/>
+        <v>-2.9077752745557879</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -990,24 +985,24 @@
         <v>6</v>
       </c>
       <c r="B19">
-        <f>80*B8</f>
+        <f t="shared" si="6"/>
         <v>626.57672978054006</v>
       </c>
       <c r="C19">
+        <f t="shared" si="9"/>
+        <v>438.60371084637802</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="7"/>
-        <v>438.60371084637802</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="8"/>
         <v>0.8834731889905616</v>
       </c>
       <c r="E19">
         <f>0.035*I8+0.00064</f>
-        <v>2.117189112930309E-3</v>
+        <v>2.060146114884033E-3</v>
       </c>
       <c r="G19">
-        <f>D19-(D8*E19)</f>
-        <v>-3.0299420315946035</v>
+        <f t="shared" si="8"/>
+        <v>-2.9245036768350987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting RVR to the MCFP formula.
</commit_message>
<xml_diff>
--- a/notes/baseline.xlsx
+++ b/notes/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="24320" yWindow="2760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>V0 (L)</t>
   </si>
   <si>
-    <t>RAP</t>
-  </si>
-  <si>
     <t>Urine Volume (mL/min)</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>SV (mL)</t>
+  </si>
+  <si>
+    <t>Slope</t>
   </si>
 </sst>
 </file>
@@ -115,8 +115,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -125,11 +127,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -462,7 +466,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -485,13 +489,13 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -503,10 +507,10 @@
         <v>4</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -818,8 +822,8 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-      <c r="G12" t="s">
-        <v>11</v>
+      <c r="F12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -835,20 +839,19 @@
         <v>205.1814504298697</v>
       </c>
       <c r="D13">
-        <f t="shared" ref="D13:D19" si="7">(B13-C13)*0.0047</f>
-        <v>0.41329406443730915</v>
+        <v>7</v>
       </c>
       <c r="E13">
-        <f>(D13-H2)/D2</f>
-        <v>4.7796610169491543E-4</v>
-      </c>
-      <c r="G13">
-        <f t="shared" ref="G13:G19" si="8">D13-(D2*E13)</f>
-        <v>0</v>
+        <f>0.035*I2 + 0.00064</f>
+        <v>3.6757586157385221E-3</v>
+      </c>
+      <c r="F13">
+        <f>24*B2</f>
+        <v>87.934907327087018</v>
       </c>
       <c r="K13">
         <f>E13*0.5/I2</f>
-        <v>2.7552937629153943E-3</v>
+        <v>2.118935788963423E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -860,24 +863,23 @@
         <v>382.3848793079091</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C19" si="9">B14*0.7</f>
+        <f t="shared" ref="C14:C19" si="7">B14*0.7</f>
         <v>267.66941551553634</v>
       </c>
       <c r="D14">
-        <f t="shared" si="7"/>
-        <v>0.539162679824152</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <f>0.035*I3+0.004045</f>
-        <v>6.372054642132057E-3</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="8"/>
-        <v>-6.6487404887373014</v>
+        <f t="shared" ref="E14:E19" si="8">0.035*I3 + 0.00064</f>
+        <v>2.9670546421320569E-3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F19" si="9">24*B3</f>
+        <v>114.71546379237273</v>
       </c>
       <c r="K14">
         <f>E13/2</f>
-        <v>2.3898305084745771E-4</v>
+        <v>1.8378793078692611E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -889,20 +891,19 @@
         <v>450.47310216858386</v>
       </c>
       <c r="C15">
+        <f t="shared" si="7"/>
+        <v>315.33117151800866</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="8"/>
+        <v>2.6153243960425599E-3</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="9"/>
-        <v>315.33117151800866</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="7"/>
-        <v>0.63516707405770345</v>
-      </c>
-      <c r="E15">
-        <f>0.035*I4+0.00064</f>
-        <v>2.6153243960425599E-3</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="8"/>
-        <v>-2.8403261428365827</v>
+        <v>135.14193065057515</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -914,23 +915,25 @@
         <v>505.5288669797514</v>
       </c>
       <c r="C16">
+        <f t="shared" si="7"/>
+        <v>353.87020688582595</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="8"/>
+        <v>2.4001972243262973E-3</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="9"/>
-        <v>353.87020688582595</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="7"/>
-        <v>0.71279570244144963</v>
-      </c>
-      <c r="E16">
-        <f>0.035*I5+0.00064</f>
-        <v>2.4001972243262973E-3</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="8"/>
-        <v>-2.8666427984163216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>151.65866009392542</v>
+      </c>
+      <c r="K16">
+        <v>2.118935788963423E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>4</v>
       </c>
@@ -939,23 +942,25 @@
         <v>551.74856346199954</v>
       </c>
       <c r="C17">
+        <f t="shared" si="7"/>
+        <v>386.22399442339963</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="8"/>
+        <v>2.2527463982710693E-3</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="9"/>
-        <v>386.22399442339963</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="7"/>
-        <v>0.77796547448141962</v>
-      </c>
-      <c r="E17">
-        <f>0.035*I6+0.00064</f>
-        <v>2.2527463982710693E-3</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="8"/>
-        <v>-2.888735813334836</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>165.52456903859988</v>
+      </c>
+      <c r="K17">
+        <v>1.8378793078692611E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>5</v>
       </c>
@@ -964,23 +969,22 @@
         <v>591.58007229244367</v>
       </c>
       <c r="C18">
+        <f t="shared" si="7"/>
+        <v>414.10605060471056</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="8"/>
+        <v>2.1441590312979552E-3</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="9"/>
-        <v>414.10605060471056</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="7"/>
-        <v>0.83412790193234565</v>
-      </c>
-      <c r="E18">
-        <f>0.035*I7+0.00064</f>
-        <v>2.1441590312979552E-3</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="8"/>
-        <v>-2.9077752745557879</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>177.47402168773311</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>6</v>
       </c>
@@ -989,24 +993,24 @@
         <v>626.57672978054006</v>
       </c>
       <c r="C19">
+        <f t="shared" si="7"/>
+        <v>438.60371084637802</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="8"/>
+        <v>2.060146114884033E-3</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="9"/>
-        <v>438.60371084637802</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="7"/>
-        <v>0.8834731889905616</v>
-      </c>
-      <c r="E19">
-        <f>0.035*I8+0.00064</f>
-        <v>2.060146114884033E-3</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="8"/>
-        <v>-2.9245036768350987</v>
+        <v>187.97301893416204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding the renal function curve.
</commit_message>
<xml_diff>
--- a/notes/baseline.xlsx
+++ b/notes/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24320" yWindow="2760" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6800" yWindow="380" windowWidth="32660" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Month</t>
   </si>
@@ -67,6 +67,27 @@
   </si>
   <si>
     <t>Slope</t>
+  </si>
+  <si>
+    <t>Renal Function (Xnormal)</t>
+  </si>
+  <si>
+    <t>Age Shift</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -98,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -115,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -123,17 +150,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -474,11 +506,14 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,14 +541,23 @@
       <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>0</v>
       </c>
@@ -545,16 +589,34 @@
         <f>(G2-H2)/D2</f>
         <v>8.673596044967205E-2</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2">
+        <v>1.3120000000000001E-6</v>
+      </c>
+      <c r="M2">
+        <f>G2+O2</f>
+        <v>137</v>
+      </c>
+      <c r="N2">
+        <f>L$2*(M2^3)+L$3*(M2^2)+L$4*M2+L$5</f>
+        <v>2.599531136</v>
+      </c>
+      <c r="O2">
+        <f>-12.5*A2+62</f>
+        <v>62</v>
+      </c>
+      <c r="Q2">
         <f>1.8*B2/60</f>
         <v>0.10991863415885877</v>
       </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L8" si="0">D2*0.088</f>
+      <c r="R2">
+        <f t="shared" ref="R2:R8" si="0">D2*0.088</f>
         <v>76.093006473705955</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1</v>
       </c>
@@ -587,16 +649,34 @@
         <f t="shared" ref="I3:I8" si="3">(G3-H3)/D3</f>
         <v>6.6487275489487338E-2</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="4">1.8*B3/60</f>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3">
+        <v>-6.6000000000000005E-5</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M5" si="4">G3+O3</f>
+        <v>124.5</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N5" si="5">L$2*(M3^3)+L$3*(M3^2)+L$4*M3+L$5</f>
+        <v>1.9311638360000003</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O8" si="6">-12.5*A3+62</f>
+        <v>49.5</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q8" si="7">1.8*B3/60</f>
         <v>0.14339432974046593</v>
       </c>
-      <c r="L3">
+      <c r="R3">
         <f t="shared" si="0"/>
         <v>99.267114668333207</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>2</v>
       </c>
@@ -605,7 +685,7 @@
         <v>5.6309137771072981</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="5">C3+1</f>
+        <f t="shared" ref="C4:C8" si="8">C3+1</f>
         <v>22</v>
       </c>
       <c r="D4">
@@ -629,16 +709,34 @@
         <f t="shared" si="3"/>
         <v>5.6437839886930283E-2</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <v>3.3890000000000001E-3</v>
+      </c>
+      <c r="M4">
         <f t="shared" si="4"/>
+        <v>112</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="5"/>
+        <v>1.3953065359999999</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="6"/>
+        <v>37</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="7"/>
         <v>0.16892741331321895</v>
       </c>
-      <c r="L4">
+      <c r="R4">
         <f t="shared" si="0"/>
         <v>116.94281732296436</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>3</v>
       </c>
@@ -647,7 +745,7 @@
         <v>6.3191108372468925</v>
       </c>
       <c r="C5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="D5">
@@ -671,16 +769,34 @@
         <f t="shared" si="3"/>
         <v>5.0291349266465626E-2</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>3.77E-4</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="4"/>
+        <v>99.5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="5"/>
+        <v>0.97658423599999999</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="6"/>
+        <v>24.5</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="7"/>
         <v>0.18957332511740679</v>
       </c>
-      <c r="L5">
+      <c r="R5">
         <f t="shared" si="0"/>
         <v>131.23529386794345</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>4</v>
       </c>
@@ -689,7 +805,7 @@
         <v>6.8968570432749949</v>
       </c>
       <c r="C6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="D6">
@@ -713,16 +829,20 @@
         <f t="shared" si="3"/>
         <v>4.6078468522030548E-2</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="4"/>
+      <c r="O6">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="7"/>
         <v>0.20690571129824986</v>
       </c>
-      <c r="L6">
+      <c r="R6">
         <f t="shared" si="0"/>
         <v>143.23392707473508</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>5</v>
       </c>
@@ -731,7 +851,7 @@
         <v>7.3947509036555461</v>
       </c>
       <c r="C7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="D7">
@@ -755,16 +875,20 @@
         <f t="shared" si="3"/>
         <v>4.2975972322798719E-2</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="4"/>
+      <c r="O7">
+        <f t="shared" si="6"/>
+        <v>-0.5</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="7"/>
         <v>0.22184252710966637</v>
       </c>
-      <c r="L7">
+      <c r="R7">
         <f t="shared" si="0"/>
         <v>153.57418676711836</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>6</v>
       </c>
@@ -773,7 +897,7 @@
         <v>7.8322091222567511</v>
       </c>
       <c r="C8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="D8">
@@ -797,16 +921,20 @@
         <f t="shared" si="3"/>
         <v>4.0575603282400931E-2</v>
       </c>
-      <c r="K8">
-        <f t="shared" si="4"/>
+      <c r="O8">
+        <f t="shared" si="6"/>
+        <v>-13</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
         <v>0.23496627366770256</v>
       </c>
-      <c r="L8">
+      <c r="R8">
         <f t="shared" si="0"/>
         <v>162.65931905102818</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -826,12 +954,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:B19" si="6">80*B2</f>
+        <f t="shared" ref="B13:B19" si="9">80*B2</f>
         <v>293.11635775695675</v>
       </c>
       <c r="C13">
@@ -849,162 +977,148 @@
         <f>24*B2</f>
         <v>87.934907327087018</v>
       </c>
-      <c r="K13">
-        <f>E13*0.5/I2</f>
-        <v>2.118935788963423E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>382.3848793079091</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C19" si="7">B14*0.7</f>
+        <f t="shared" ref="C14:C19" si="10">B14*0.7</f>
         <v>267.66941551553634</v>
       </c>
       <c r="D14">
         <v>7</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:E19" si="8">0.035*I3 + 0.00064</f>
+        <f t="shared" ref="E14:E19" si="11">0.035*I3 + 0.00064</f>
         <v>2.9670546421320569E-3</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:F19" si="9">24*B3</f>
+        <f t="shared" ref="F14:F19" si="12">24*B3</f>
         <v>114.71546379237273</v>
       </c>
-      <c r="K14">
-        <f>E13/2</f>
-        <v>1.8378793078692611E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>450.47310216858386</v>
       </c>
       <c r="C15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>315.33117151800866</v>
       </c>
       <c r="D15">
         <v>7</v>
       </c>
       <c r="E15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.6153243960425599E-3</v>
       </c>
       <c r="F15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>135.14193065057515</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>3</v>
       </c>
       <c r="B16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>505.5288669797514</v>
       </c>
       <c r="C16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>353.87020688582595</v>
       </c>
       <c r="D16">
         <v>7</v>
       </c>
       <c r="E16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.4001972243262973E-3</v>
       </c>
       <c r="F16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>151.65866009392542</v>
       </c>
-      <c r="K16">
-        <v>2.118935788963423E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>551.74856346199954</v>
       </c>
       <c r="C17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>386.22399442339963</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
       <c r="E17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.2527463982710693E-3</v>
       </c>
       <c r="F17">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>165.52456903859988</v>
       </c>
-      <c r="K17">
-        <v>1.8378793078692611E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>591.58007229244367</v>
       </c>
       <c r="C18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>414.10605060471056</v>
       </c>
       <c r="D18">
         <v>7</v>
       </c>
       <c r="E18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.1441590312979552E-3</v>
       </c>
       <c r="F18">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>177.47402168773311</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>6</v>
       </c>
       <c r="B19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>626.57672978054006</v>
       </c>
       <c r="C19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>438.60371084637802</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
       <c r="E19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>2.060146114884033E-3</v>
       </c>
       <c r="F19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>187.97301893416204</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding the RVR functions.
</commit_message>
<xml_diff>
--- a/notes/baseline.xlsx
+++ b/notes/baseline.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="380" windowWidth="32660" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="6795" yWindow="375" windowWidth="32655" windowHeight="15870" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Month</t>
   </si>
@@ -88,13 +88,22 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>RVR/2</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>constant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -494,23 +503,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" customWidth="1"/>
-    <col min="14" max="14" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.125" customWidth="1"/>
+    <col min="14" max="14" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -953,6 +964,12 @@
       <c r="F12" t="s">
         <v>15</v>
       </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13">
@@ -977,6 +994,9 @@
         <f>24*B2</f>
         <v>87.934907327087018</v>
       </c>
+      <c r="K13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14">
@@ -1001,6 +1021,21 @@
         <f t="shared" ref="F14:F19" si="12">24*B3</f>
         <v>114.71546379237273</v>
       </c>
+      <c r="H14">
+        <f>D14/D3</f>
+        <v>6.2054790456854848E-3</v>
+      </c>
+      <c r="I14">
+        <f>H14/2</f>
+        <v>3.1027395228427424E-3</v>
+      </c>
+      <c r="K14">
+        <f t="array" ref="K14:L18">LINEST(I14:I19,I3:I8,TRUE,TRUE)</f>
+        <v>4.6666666666666676E-2</v>
+      </c>
+      <c r="L14">
+        <v>-1.3010426069826053E-18</v>
+      </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15">
@@ -1025,6 +1060,20 @@
         <f t="shared" si="12"/>
         <v>135.14193065057515</v>
       </c>
+      <c r="H15">
+        <f>D15/D4</f>
+        <v>5.2675317227801602E-3</v>
+      </c>
+      <c r="I15">
+        <f>H15/2</f>
+        <v>2.6337658613900801E-3</v>
+      </c>
+      <c r="K15">
+        <v>7.7439260063963266E-18</v>
+      </c>
+      <c r="L15">
+        <v>3.9677762011799429E-19</v>
+      </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16">
@@ -1049,8 +1098,22 @@
         <f t="shared" si="12"/>
         <v>151.65866009392542</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16">
+        <f>D16/D5</f>
+        <v>4.6938592648701248E-3</v>
+      </c>
+      <c r="I16">
+        <f>H16/2</f>
+        <v>2.3469296324350624E-3</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1.6708677635297571E-19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1073,8 +1136,22 @@
         <f t="shared" si="12"/>
         <v>165.52456903859988</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17">
+        <f>D17/D6</f>
+        <v>4.3006570620561842E-3</v>
+      </c>
+      <c r="I17">
+        <f>H17/2</f>
+        <v>2.1503285310280921E-3</v>
+      </c>
+      <c r="K17">
+        <v>3.6315428479047731E+31</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1097,8 +1174,22 @@
         <f t="shared" si="12"/>
         <v>177.47402168773311</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18">
+        <f>D18/D7</f>
+        <v>4.0110907501278801E-3</v>
+      </c>
+      <c r="I18">
+        <f>H18/2</f>
+        <v>2.00554537506394E-3</v>
+      </c>
+      <c r="K18">
+        <v>1.0138537993392714E-6</v>
+      </c>
+      <c r="L18">
+        <v>1.1167196332811731E-37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1120,6 +1211,60 @@
       <c r="F19">
         <f t="shared" si="12"/>
         <v>187.97301893416204</v>
+      </c>
+      <c r="H19">
+        <f>D19/D8</f>
+        <v>3.7870563063574204E-3</v>
+      </c>
+      <c r="I19">
+        <f>H19/2</f>
+        <v>1.8935281531787102E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="K21">
+        <f t="array" ref="K21:L25">LINEST(I14:I19,A3:A8,TRUE,TRUE)</f>
+        <v>-2.3220912596301572E-4</v>
+      </c>
+      <c r="L21">
+        <v>3.168204786860326E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="K22">
+        <v>3.1675797696661144E-5</v>
+      </c>
+      <c r="L22">
+        <v>1.233595088447462E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="K23">
+        <v>0.93072479362787974</v>
+      </c>
+      <c r="L23">
+        <v>1.325093687068826E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="K24">
+        <v>53.740715754977465</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="K25">
+        <v>9.4361886815888517E-7</v>
+      </c>
+      <c r="L25">
+        <v>7.0234931180386235E-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>